<commit_message>
create stop, restart, reset button
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박지우\Desktop\바코드\실행파일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parkjiwoo/Desktop/Orange_board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A298D312-1510-44C6-842B-994DF77D6770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E1DFE6-39EA-B947-8463-F1A9562001C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="420" windowWidth="18615" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="500" windowWidth="14820" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,22 +52,19 @@
   </si>
   <si>
     <t>a880167555826</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>a02403964220</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>a02403964220</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a978895940627</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +79,13 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,8 +114,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,16 +400,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="27.75" customWidth="1"/>
-    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,18 +420,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -438,12 +442,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Revert "create stop, restart, reset button"
This reverts commit 40439e4abe8edc40a8dca2f02a35226a09f53923.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parkjiwoo/Desktop/Orange_board/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박지우\Desktop\바코드\실행파일\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E1DFE6-39EA-B947-8463-F1A9562001C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A298D312-1510-44C6-842B-994DF77D6770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="500" windowWidth="14820" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="18615" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,19 +52,22 @@
   </si>
   <si>
     <t>a880167555826</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>a02403964220</t>
-  </si>
-  <si>
-    <t>a978895940627</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a02403964220</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,13 +82,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Malgun Gothic"/>
-      <family val="2"/>
-      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,8 +110,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,16 +396,16 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.75" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,18 +416,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -442,12 +438,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>

</xml_diff>